<commit_message>
Add US for the following domains: Computer Networks and Computer Vision
</commit_message>
<xml_diff>
--- a/refair-server/datasets/Few Shot dataset/FSDataset3.xlsx
+++ b/refair-server/datasets/Few Shot dataset/FSDataset3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele\Desktop\SE4AI Project\US mie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele\Desktop\SE4AI Project\ReFair-App\refair-server\datasets\Few Shot dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CDF0BB-FE10-4188-AA1A-419081D838E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD895AC4-54AD-47A7-B362-F66ADDF5F23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="134">
   <si>
     <t>Domain cluster</t>
   </si>
@@ -318,6 +318,126 @@
   </si>
   <si>
     <t>As a sports marketing manager, I want to leverage word embedding techniques to analyze social media discussions and fan sentiments around sporting events and athletes, to optimize marketing campaigns and sponsorship strategies for maximum audience engagement and brand impact.</t>
+  </si>
+  <si>
+    <t>As a network security analyst, I want to apply adversarial learning techniques to detect and mitigate adversarial attacks on network traffic, so that I can enhance the resilience of our network infrastructure against sophisticated cyber threats.</t>
+  </si>
+  <si>
+    <t>As a computer vision engineer, I want to integrate adversarial training into our image classification system to mitigate the impact of adversarial examples, thereby improving the model's accuracy and reliability in critical applications.</t>
+  </si>
+  <si>
+    <t>As a network administrator, I want to utilize CNNs for anomaly detection in network traffic behavior, so that I can quickly identify and mitigate unusual activities that could indicate security breaches or faults.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to develop a CNN-based object detection system that accurately localizes and identifies multiple objects within images, allowing me to enhance surveillance systems and automate inventory management processes.</t>
+  </si>
+  <si>
+    <t>As a network engineer, I want a conversational agent powered by NLP to assist in troubleshooting network issues, so that I can quickly identify and resolve connectivity problems across our infrastructure.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want a conversational agent to provide me with real-time updates on the latest advancements and research papers in image classification, so that I can stay informed about cutting-edge techniques and methodologies.</t>
+  </si>
+  <si>
+    <t>As a network engineer, I want to employ decision tree algorithms to analyze network traffic patterns and classify different types of network attacks, so that I can enhance our intrusion detection and prevention systems.</t>
+  </si>
+  <si>
+    <t>As a remote sensing analyst, I seek to utilize decision tree algorithms to detect anomalies such as deforestation patches or infrastructure changes in satellite imagery, enabling proactive monitoring and timely interventions for environmental conservation or urban planning purposes.</t>
+  </si>
+  <si>
+    <t>As a cybersecurity analyst, I want to leverage document classification in NLP to classify security incident reports based on their content, so that I can prioritize and respond to threats effectively.</t>
+  </si>
+  <si>
+    <t>As a digital librarian managing a large database of scanned books, I want to employ document classification to classify novels, textbooks, and reference materials into distinct genres and subjects, enabling readers to quickly find and borrow books of interest from our digital collection.</t>
+  </si>
+  <si>
+    <t>As a cybersecurity analyst, I want to utilize entity extraction in NLP to detect and extract mentions of potential security threats, such as IP addresses, domain names, and malware types, from network security alerts and incident reports, so that I can promptly investigate and mitigate security breaches.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I need entity extraction to extract relevant entities such as landmarks, buildings, and geographic features from textual descriptions associated with satellite images, aiding in geospatial analysis and urban planning.</t>
+  </si>
+  <si>
+    <t>As a network analyst, I want to employ feature selection techniques in machine learning to identify the most relevant network traffic parameters, so that I can build more efficient intrusion detection systems and enhance network security.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to perform feature selection to identify the most discriminative visual features in image datasets, so that I can improve the accuracy of object recognition models and reduce computational overhead.</t>
+  </si>
+  <si>
+    <t>As a network security analyst, I want to employ techniques for handling imbalanced datasets in machine learning to better detect rare and critical cybersecurity threats, such as zero-day attacks, so that our network remains secure against evolving threats.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to address class imbalance in my dataset so that my model can accurately detect rare visual anomalies in industrial inspection images, ensuring early detection of critical faults and minimizing downtime."</t>
+  </si>
+  <si>
+    <t>As a network security analyst, I want to apply keyword extraction in NLP to analyze security incident reports and identify key terms related to potential threats, so that I can prioritize and respond to security incidents effectively.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to implement keyword extraction to automatically identify and extract relevant keywords from image captions and metadata, so that I can improve image search accuracy and retrieval efficiency.</t>
+  </si>
+  <si>
+    <t>As a network engineer, I want to utilize k-nearest neighbor to classify network traffic patterns, so that I can optimize Quality of Service (QoS) parameters and ensure efficient data transmission across different network segments.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to implement a k-nearest neighbor algorithm to classify images based on their features (such as color histograms or texture descriptors), so that I can automatically categorize large datasets of images into predefined classes.</t>
+  </si>
+  <si>
+    <t>As a network engineer, I want to leverage multi-label classification in NLP to automatically categorize network security alerts based on their severity and type, so that I can prioritize and respond to critical incidents more efficiently.</t>
+  </si>
+  <si>
+    <t>As a Computer Vision researcher, I want to use multi-label classification to automatically tag images with relevant categories such as "sunset," "beach," "nature," and "landscape," based on their visual content, to improve image retrieval and organization in large datasets.</t>
+  </si>
+  <si>
+    <t>As a network administrator, I want to employ neural networks for traffic prediction and optimization, so that I can efficiently manage bandwidth allocation and improve overall network performance during peak usage times.</t>
+  </si>
+  <si>
+    <t>As a medical imaging specialist, I need to employ neural networks for precise image segmentation of MRI scans, enabling me to accurately identify and analyze different tissues and abnormalities for diagnostic purposes.</t>
+  </si>
+  <si>
+    <t>As a network administrator, I want to utilize Random Forest algorithms for anomaly detection in network logs and traffic flows, so that I can swiftly identify and mitigate potential network breaches or operational issues.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to use Random Forest to preprocess image data by extracting relevant features such as textures, edges, and colors, so that I can prepare high-quality input for subsequent computer vision algorithms.</t>
+  </si>
+  <si>
+    <t>As a network operations manager, I want to apply semantic similarity algorithms in NLP to classify and group similar network troubleshooting tickets automatically, so that I can prioritize and resolve network issues more efficiently.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to use semantic similarity techniques in NLP to match textual descriptions of images with similar visual content, enabling efficient retrieval of relevant images from large datasets.</t>
+  </si>
+  <si>
+    <t>As a researcher in network traffic analysis, I want to explore sentiment analysis techniques on user forums and discussion boards to gauge public sentiment towards emerging network technologies, so that we can anticipate adoption trends and user preferences.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to implement sentiment analysis on textual comments associated with images, so that I can automatically classify the emotional response elicited by visual content.</t>
+  </si>
+  <si>
+    <t>As a cybersecurity analyst, I want to leverage speech-to-text algorithms to transcribe real-time network security incident response calls accurately, enabling quicker analysis and decision-making during critical events.</t>
+  </si>
+  <si>
+    <t>As a video analytics developer, I want to integrate a speech-to-text model capable of identifying and transcribing multiple languages spoken within security camera feeds, facilitating real-time monitoring and threat detection across diverse linguistic environments.</t>
+  </si>
+  <si>
+    <t>As a network security analyst, I want to utilize text categorization techniques in NLP to automatically classify network log messages into predefined categories (such as intrusion, system error, or normal operation), so that I can quickly identify and respond to security incidents more effectively.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to employ text categorization to automatically identify the language used in image captions and embedded text, enabling better content localization and user engagement across diverse global audiences.</t>
+  </si>
+  <si>
+    <t>As a network administrator, I want to apply unsupervised clustering techniques to network traffic data, so that I can identify patterns of communication and detect potential anomalies or cyber threats more effectively.</t>
+  </si>
+  <si>
+    <t>As a security analyst, I want to apply unsupervised clustering techniques to detect anomalies in surveillance footage, identifying unusual activities or objects that require further investigation.</t>
+  </si>
+  <si>
+    <t>As a telecommunications engineer, I want to integrate voice recognition into network troubleshooting tools, so that I can verbally query and receive detailed diagnostic reports on network issues, enhancing efficiency in resolving connectivity problems.</t>
+  </si>
+  <si>
+    <t>As a video analytics researcher, I want to deploy voice recognition capabilities to extract spoken content from CCTV recordings, allowing for automated analysis of conversations and detection of suspicious activities or anomalies.</t>
+  </si>
+  <si>
+    <t>As a network researcher, I want to leverage word embedding methods in NLP to predict network traffic trends and bandwidth requirements from textual data, so that I can optimize network resource allocation and capacity planning.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to leverage word embedding techniques to enhance image captioning models, so that they can generate more contextually accurate and semantically rich descriptions of visual content.</t>
   </si>
 </sst>
 </file>
@@ -401,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -429,8 +549,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -774,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
   <dimension ref="A1:F381"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="B85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2007,2549 +2126,2029 @@
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="15" t="s">
+    <row r="62" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A62" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B62" s="16">
-        <v>9</v>
-      </c>
-      <c r="C62" s="15" t="s">
+      <c r="B62" s="15">
+        <v>9</v>
+      </c>
+      <c r="C62" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E62" s="1"/>
+      <c r="E62" t="s">
+        <v>94</v>
+      </c>
       <c r="F62" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="15" t="s">
+    <row r="63" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A63" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B63" s="16">
-        <v>9</v>
-      </c>
-      <c r="C63" s="15" t="s">
+      <c r="B63" s="15">
+        <v>9</v>
+      </c>
+      <c r="C63" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E63" s="1"/>
+      <c r="E63" t="s">
+        <v>95</v>
+      </c>
       <c r="F63" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="15" t="s">
+    <row r="64" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A64" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B64" s="16">
-        <v>9</v>
-      </c>
-      <c r="C64" s="15" t="s">
+      <c r="B64" s="15">
+        <v>9</v>
+      </c>
+      <c r="C64" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E64" s="1"/>
+      <c r="E64" t="s">
+        <v>96</v>
+      </c>
       <c r="F64" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
+    <row r="65" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A65" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B65" s="16">
-        <v>9</v>
-      </c>
-      <c r="C65" s="15" t="s">
+      <c r="B65" s="15">
+        <v>9</v>
+      </c>
+      <c r="C65" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E65" s="1"/>
+      <c r="E65" t="s">
+        <v>97</v>
+      </c>
       <c r="F65" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="15" t="s">
+    <row r="66" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A66" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B66" s="16">
-        <v>9</v>
-      </c>
-      <c r="C66" s="15" t="s">
+      <c r="B66" s="15">
+        <v>9</v>
+      </c>
+      <c r="C66" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E66" s="1"/>
+      <c r="E66" t="s">
+        <v>98</v>
+      </c>
       <c r="F66" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="15" t="s">
+    <row r="67" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A67" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B67" s="16">
-        <v>9</v>
-      </c>
-      <c r="C67" s="15" t="s">
+      <c r="B67" s="15">
+        <v>9</v>
+      </c>
+      <c r="C67" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E67" s="1"/>
+      <c r="E67" t="s">
+        <v>99</v>
+      </c>
       <c r="F67" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="68" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="15" t="s">
+    <row r="68" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A68" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B68" s="16">
-        <v>9</v>
-      </c>
-      <c r="C68" s="15" t="s">
+      <c r="B68" s="15">
+        <v>9</v>
+      </c>
+      <c r="C68" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E68" s="1"/>
+      <c r="E68" t="s">
+        <v>100</v>
+      </c>
       <c r="F68" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="15" t="s">
+    <row r="69" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A69" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B69" s="16">
-        <v>9</v>
-      </c>
-      <c r="C69" s="15" t="s">
+      <c r="B69" s="15">
+        <v>9</v>
+      </c>
+      <c r="C69" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E69" s="1"/>
+      <c r="E69" t="s">
+        <v>101</v>
+      </c>
       <c r="F69" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="15" t="s">
+    <row r="70" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A70" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B70" s="16">
-        <v>9</v>
-      </c>
-      <c r="C70" s="15" t="s">
+      <c r="B70" s="15">
+        <v>9</v>
+      </c>
+      <c r="C70" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E70" s="1"/>
+      <c r="E70" t="s">
+        <v>102</v>
+      </c>
       <c r="F70" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="15" t="s">
+    <row r="71" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A71" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B71" s="16">
-        <v>9</v>
-      </c>
-      <c r="C71" s="15" t="s">
+      <c r="B71" s="15">
+        <v>9</v>
+      </c>
+      <c r="C71" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E71" s="1"/>
+      <c r="E71" t="s">
+        <v>103</v>
+      </c>
       <c r="F71" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="15" t="s">
+    <row r="72" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A72" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B72" s="16">
-        <v>9</v>
-      </c>
-      <c r="C72" s="15" t="s">
+      <c r="B72" s="15">
+        <v>9</v>
+      </c>
+      <c r="C72" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E72" s="1"/>
+      <c r="E72" t="s">
+        <v>104</v>
+      </c>
       <c r="F72" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="15" t="s">
+    <row r="73" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A73" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B73" s="16">
-        <v>9</v>
-      </c>
-      <c r="C73" s="15" t="s">
+      <c r="B73" s="15">
+        <v>9</v>
+      </c>
+      <c r="C73" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E73" s="1"/>
+      <c r="E73" t="s">
+        <v>105</v>
+      </c>
       <c r="F73" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="15" t="s">
+    <row r="74" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A74" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B74" s="16">
-        <v>9</v>
-      </c>
-      <c r="C74" s="15" t="s">
+      <c r="B74" s="15">
+        <v>9</v>
+      </c>
+      <c r="C74" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E74" s="1"/>
+      <c r="E74" t="s">
+        <v>106</v>
+      </c>
       <c r="F74" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="15" t="s">
+    <row r="75" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A75" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B75" s="16">
-        <v>9</v>
-      </c>
-      <c r="C75" s="15" t="s">
+      <c r="B75" s="15">
+        <v>9</v>
+      </c>
+      <c r="C75" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E75" s="1"/>
+      <c r="E75" t="s">
+        <v>107</v>
+      </c>
       <c r="F75" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="15" t="s">
+    <row r="76" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A76" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B76" s="16">
-        <v>9</v>
-      </c>
-      <c r="C76" s="15" t="s">
+      <c r="B76" s="15">
+        <v>9</v>
+      </c>
+      <c r="C76" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E76" s="1"/>
+      <c r="E76" t="s">
+        <v>108</v>
+      </c>
       <c r="F76" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="15" t="s">
+    <row r="77" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A77" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B77" s="16">
-        <v>9</v>
-      </c>
-      <c r="C77" s="15" t="s">
+      <c r="B77" s="15">
+        <v>9</v>
+      </c>
+      <c r="C77" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E77" s="1"/>
+      <c r="E77" t="s">
+        <v>109</v>
+      </c>
       <c r="F77" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="15" t="s">
+    <row r="78" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A78" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B78" s="16">
-        <v>9</v>
-      </c>
-      <c r="C78" s="15" t="s">
+      <c r="B78" s="15">
+        <v>9</v>
+      </c>
+      <c r="C78" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E78" s="1"/>
+      <c r="E78" t="s">
+        <v>110</v>
+      </c>
       <c r="F78" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="15" t="s">
+    <row r="79" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A79" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B79" s="16">
-        <v>9</v>
-      </c>
-      <c r="C79" s="15" t="s">
+      <c r="B79" s="15">
+        <v>9</v>
+      </c>
+      <c r="C79" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E79" s="1"/>
+      <c r="E79" t="s">
+        <v>111</v>
+      </c>
       <c r="F79" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="15" t="s">
+    <row r="80" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A80" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B80" s="16">
-        <v>9</v>
-      </c>
-      <c r="C80" s="15" t="s">
+      <c r="B80" s="15">
+        <v>9</v>
+      </c>
+      <c r="C80" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E80" s="1"/>
+      <c r="E80" t="s">
+        <v>112</v>
+      </c>
       <c r="F80" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="15" t="s">
+    <row r="81" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A81" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B81" s="16">
-        <v>9</v>
-      </c>
-      <c r="C81" s="15" t="s">
+      <c r="B81" s="15">
+        <v>9</v>
+      </c>
+      <c r="C81" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E81" s="1"/>
+      <c r="E81" t="s">
+        <v>113</v>
+      </c>
       <c r="F81" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="15" t="s">
+    <row r="82" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A82" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B82" s="16">
-        <v>9</v>
-      </c>
-      <c r="C82" s="15" t="s">
+      <c r="B82" s="15">
+        <v>9</v>
+      </c>
+      <c r="C82" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E82" s="1"/>
+      <c r="E82" t="s">
+        <v>114</v>
+      </c>
       <c r="F82" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="15" t="s">
+    <row r="83" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A83" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B83" s="16">
-        <v>9</v>
-      </c>
-      <c r="C83" s="15" t="s">
+      <c r="B83" s="15">
+        <v>9</v>
+      </c>
+      <c r="C83" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E83" s="1"/>
+      <c r="E83" t="s">
+        <v>115</v>
+      </c>
       <c r="F83" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="15" t="s">
+    <row r="84" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A84" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B84" s="16">
-        <v>9</v>
-      </c>
-      <c r="C84" s="15" t="s">
+      <c r="B84" s="15">
+        <v>9</v>
+      </c>
+      <c r="C84" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E84" s="1"/>
+      <c r="E84" t="s">
+        <v>116</v>
+      </c>
       <c r="F84" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="15" t="s">
+    <row r="85" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A85" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B85" s="16">
-        <v>9</v>
-      </c>
-      <c r="C85" s="15" t="s">
+      <c r="B85" s="15">
+        <v>9</v>
+      </c>
+      <c r="C85" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E85" s="1"/>
+      <c r="E85" t="s">
+        <v>117</v>
+      </c>
       <c r="F85" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="15" t="s">
+    <row r="86" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A86" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B86" s="16">
-        <v>9</v>
-      </c>
-      <c r="C86" s="15" t="s">
+      <c r="B86" s="15">
+        <v>9</v>
+      </c>
+      <c r="C86" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E86" s="1"/>
+      <c r="E86" t="s">
+        <v>118</v>
+      </c>
       <c r="F86" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="15" t="s">
+    <row r="87" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A87" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B87" s="16">
-        <v>9</v>
-      </c>
-      <c r="C87" s="15" t="s">
+      <c r="B87" s="15">
+        <v>9</v>
+      </c>
+      <c r="C87" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D87" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E87" s="1"/>
+      <c r="E87" t="s">
+        <v>119</v>
+      </c>
       <c r="F87" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="15" t="s">
+    <row r="88" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A88" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B88" s="16">
-        <v>9</v>
-      </c>
-      <c r="C88" s="15" t="s">
+      <c r="B88" s="15">
+        <v>9</v>
+      </c>
+      <c r="C88" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D88" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E88" s="1"/>
+      <c r="E88" t="s">
+        <v>120</v>
+      </c>
       <c r="F88" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="15" t="s">
+    <row r="89" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A89" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B89" s="16">
-        <v>9</v>
-      </c>
-      <c r="C89" s="15" t="s">
+      <c r="B89" s="15">
+        <v>9</v>
+      </c>
+      <c r="C89" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E89" s="1"/>
+      <c r="E89" t="s">
+        <v>121</v>
+      </c>
       <c r="F89" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="15" t="s">
+    <row r="90" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A90" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B90" s="16">
-        <v>9</v>
-      </c>
-      <c r="C90" s="15" t="s">
+      <c r="B90" s="15">
+        <v>9</v>
+      </c>
+      <c r="C90" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D90" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E90" s="1"/>
+      <c r="E90" t="s">
+        <v>122</v>
+      </c>
       <c r="F90" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="15" t="s">
+    <row r="91" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A91" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B91" s="16">
-        <v>9</v>
-      </c>
-      <c r="C91" s="15" t="s">
+      <c r="B91" s="15">
+        <v>9</v>
+      </c>
+      <c r="C91" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E91" s="1"/>
+      <c r="E91" t="s">
+        <v>123</v>
+      </c>
       <c r="F91" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="92" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="15" t="s">
+    <row r="92" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A92" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B92" s="16">
-        <v>9</v>
-      </c>
-      <c r="C92" s="15" t="s">
+      <c r="B92" s="15">
+        <v>9</v>
+      </c>
+      <c r="C92" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D92" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E92" s="1"/>
+      <c r="E92" t="s">
+        <v>124</v>
+      </c>
       <c r="F92" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="15" t="s">
+    <row r="93" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A93" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B93" s="16">
-        <v>9</v>
-      </c>
-      <c r="C93" s="15" t="s">
+      <c r="B93" s="15">
+        <v>9</v>
+      </c>
+      <c r="C93" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D93" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E93" s="1"/>
+      <c r="E93" t="s">
+        <v>125</v>
+      </c>
       <c r="F93" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="15" t="s">
+    <row r="94" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A94" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B94" s="16">
-        <v>9</v>
-      </c>
-      <c r="C94" s="15" t="s">
+      <c r="B94" s="15">
+        <v>9</v>
+      </c>
+      <c r="C94" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E94" s="1"/>
+      <c r="E94" t="s">
+        <v>126</v>
+      </c>
       <c r="F94" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="15" t="s">
+    <row r="95" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A95" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B95" s="16">
-        <v>9</v>
-      </c>
-      <c r="C95" s="15" t="s">
+      <c r="B95" s="15">
+        <v>9</v>
+      </c>
+      <c r="C95" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D95" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E95" s="1"/>
+      <c r="E95" t="s">
+        <v>127</v>
+      </c>
       <c r="F95" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="96" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="15" t="s">
+    <row r="96" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A96" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B96" s="16">
-        <v>9</v>
-      </c>
-      <c r="C96" s="15" t="s">
+      <c r="B96" s="15">
+        <v>9</v>
+      </c>
+      <c r="C96" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E96" s="1"/>
+      <c r="E96" t="s">
+        <v>128</v>
+      </c>
       <c r="F96" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="15" t="s">
+    <row r="97" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A97" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B97" s="16">
-        <v>9</v>
-      </c>
-      <c r="C97" s="15" t="s">
+      <c r="B97" s="15">
+        <v>9</v>
+      </c>
+      <c r="C97" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E97" s="1"/>
+      <c r="E97" t="s">
+        <v>129</v>
+      </c>
       <c r="F97" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="15" t="s">
+    <row r="98" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A98" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B98" s="16">
-        <v>9</v>
-      </c>
-      <c r="C98" s="15" t="s">
+      <c r="B98" s="15">
+        <v>9</v>
+      </c>
+      <c r="C98" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E98" s="1"/>
+      <c r="E98" t="s">
+        <v>130</v>
+      </c>
       <c r="F98" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="15" t="s">
+    <row r="99" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A99" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B99" s="16">
-        <v>9</v>
-      </c>
-      <c r="C99" s="15" t="s">
+      <c r="B99" s="15">
+        <v>9</v>
+      </c>
+      <c r="C99" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E99" s="1"/>
+      <c r="E99" t="s">
+        <v>131</v>
+      </c>
       <c r="F99" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="100" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="15" t="s">
+    <row r="100" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A100" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B100" s="16">
-        <v>9</v>
-      </c>
-      <c r="C100" s="15" t="s">
+      <c r="B100" s="15">
+        <v>9</v>
+      </c>
+      <c r="C100" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E100" s="1"/>
+      <c r="E100" t="s">
+        <v>132</v>
+      </c>
       <c r="F100" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="101" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="15" t="s">
+    <row r="101" spans="1:6" s="2" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A101" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B101" s="16">
-        <v>9</v>
-      </c>
-      <c r="C101" s="15" t="s">
+      <c r="B101" s="15">
+        <v>9</v>
+      </c>
+      <c r="C101" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E101" s="1"/>
+      <c r="E101" t="s">
+        <v>133</v>
+      </c>
       <c r="F101" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="102" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="13"/>
-      <c r="B102" s="13"/>
-      <c r="C102" s="13"/>
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
       <c r="D102" s="3"/>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
     </row>
     <row r="103" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="13"/>
-      <c r="B103" s="13"/>
-      <c r="C103" s="13"/>
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
       <c r="D103" s="3"/>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
     </row>
     <row r="104" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="13"/>
-      <c r="B104" s="13"/>
-      <c r="C104" s="13"/>
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
       <c r="D104" s="3"/>
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
     </row>
     <row r="105" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="13"/>
-      <c r="B105" s="13"/>
-      <c r="C105" s="13"/>
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
       <c r="D105" s="3"/>
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
     </row>
     <row r="106" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="13"/>
-      <c r="B106" s="13"/>
-      <c r="C106" s="13"/>
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
       <c r="D106" s="3"/>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
     </row>
     <row r="107" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="13"/>
-      <c r="B107" s="13"/>
-      <c r="C107" s="13"/>
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
       <c r="D107" s="3"/>
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
     </row>
     <row r="108" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="13"/>
-      <c r="B108" s="13"/>
-      <c r="C108" s="13"/>
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
       <c r="D108" s="3"/>
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
     </row>
     <row r="109" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="13"/>
-      <c r="B109" s="13"/>
-      <c r="C109" s="13"/>
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
       <c r="D109" s="3"/>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
     </row>
     <row r="110" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="13"/>
-      <c r="B110" s="13"/>
-      <c r="C110" s="13"/>
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
       <c r="D110" s="3"/>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
     </row>
     <row r="111" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="13"/>
-      <c r="B111" s="13"/>
-      <c r="C111" s="13"/>
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
       <c r="D111" s="3"/>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
     </row>
     <row r="112" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="13"/>
-      <c r="B112" s="13"/>
-      <c r="C112" s="13"/>
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
       <c r="D112" s="3"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
     </row>
     <row r="113" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="13"/>
-      <c r="B113" s="13"/>
-      <c r="C113" s="13"/>
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
       <c r="D113" s="3"/>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
     </row>
     <row r="114" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="13"/>
-      <c r="B114" s="13"/>
-      <c r="C114" s="13"/>
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
       <c r="D114" s="3"/>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
     </row>
     <row r="115" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="13"/>
-      <c r="B115" s="13"/>
-      <c r="C115" s="13"/>
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="1"/>
       <c r="D115" s="3"/>
       <c r="E115" s="5"/>
       <c r="F115" s="1"/>
     </row>
     <row r="116" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="13"/>
-      <c r="B116" s="13"/>
-      <c r="C116" s="13"/>
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="1"/>
       <c r="D116" s="3"/>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
     </row>
     <row r="117" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="13"/>
-      <c r="B117" s="13"/>
-      <c r="C117" s="13"/>
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+      <c r="C117" s="1"/>
       <c r="D117" s="3"/>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
     </row>
     <row r="118" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="13"/>
-      <c r="B118" s="13"/>
-      <c r="C118" s="13"/>
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+      <c r="C118" s="1"/>
       <c r="D118" s="3"/>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
     </row>
     <row r="119" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="13"/>
-      <c r="B119" s="13"/>
-      <c r="C119" s="13"/>
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+      <c r="C119" s="1"/>
       <c r="D119" s="3"/>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
     </row>
     <row r="120" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="13"/>
-      <c r="B120" s="13"/>
-      <c r="C120" s="13"/>
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+      <c r="C120" s="1"/>
       <c r="D120" s="3"/>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
     </row>
     <row r="121" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="13"/>
-      <c r="B121" s="13"/>
-      <c r="C121" s="13"/>
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
+      <c r="C121" s="1"/>
       <c r="D121" s="3"/>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="14"/>
-      <c r="B122" s="14"/>
-      <c r="C122" s="14"/>
+      <c r="A122" s="13"/>
+      <c r="B122" s="13"/>
+      <c r="C122" s="13"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="14"/>
-      <c r="B123" s="14"/>
-      <c r="C123" s="14"/>
+      <c r="A123" s="13"/>
+      <c r="B123" s="13"/>
+      <c r="C123" s="13"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="14"/>
-      <c r="B124" s="14"/>
-      <c r="C124" s="14"/>
+      <c r="A124" s="13"/>
+      <c r="B124" s="13"/>
+      <c r="C124" s="13"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="14"/>
-      <c r="B125" s="14"/>
-      <c r="C125" s="14"/>
+      <c r="A125" s="13"/>
+      <c r="B125" s="13"/>
+      <c r="C125" s="13"/>
       <c r="E125" s="5"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="14"/>
-      <c r="B126" s="14"/>
-      <c r="C126" s="14"/>
+      <c r="A126" s="13"/>
+      <c r="B126" s="13"/>
+      <c r="C126" s="13"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="14"/>
-      <c r="B127" s="14"/>
-      <c r="C127" s="14"/>
+      <c r="A127" s="13"/>
+      <c r="B127" s="13"/>
+      <c r="C127" s="13"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="14"/>
-      <c r="B128" s="14"/>
-      <c r="C128" s="14"/>
+      <c r="A128" s="13"/>
+      <c r="B128" s="13"/>
+      <c r="C128" s="13"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" s="14"/>
-      <c r="B129" s="14"/>
-      <c r="C129" s="14"/>
+      <c r="A129" s="13"/>
+      <c r="B129" s="13"/>
+      <c r="C129" s="13"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" s="14"/>
-      <c r="B130" s="14"/>
-      <c r="C130" s="14"/>
+      <c r="A130" s="13"/>
+      <c r="B130" s="13"/>
+      <c r="C130" s="13"/>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" s="14"/>
-      <c r="B131" s="14"/>
-      <c r="C131" s="14"/>
+      <c r="A131" s="13"/>
+      <c r="B131" s="13"/>
+      <c r="C131" s="13"/>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" s="14"/>
-      <c r="B132" s="14"/>
-      <c r="C132" s="14"/>
+      <c r="A132" s="13"/>
+      <c r="B132" s="13"/>
+      <c r="C132" s="13"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" s="14"/>
-      <c r="B133" s="14"/>
-      <c r="C133" s="14"/>
+      <c r="A133" s="13"/>
+      <c r="B133" s="13"/>
+      <c r="C133" s="13"/>
       <c r="E133" s="5"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" s="14"/>
-      <c r="B134" s="14"/>
-      <c r="C134" s="14"/>
+      <c r="A134" s="13"/>
+      <c r="B134" s="13"/>
+      <c r="C134" s="13"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" s="14"/>
-      <c r="B135" s="14"/>
-      <c r="C135" s="14"/>
+      <c r="A135" s="13"/>
+      <c r="B135" s="13"/>
+      <c r="C135" s="13"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" s="14"/>
-      <c r="B136" s="14"/>
-      <c r="C136" s="14"/>
+      <c r="A136" s="13"/>
+      <c r="B136" s="13"/>
+      <c r="C136" s="13"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" s="14"/>
-      <c r="B137" s="14"/>
-      <c r="C137" s="14"/>
+      <c r="A137" s="13"/>
+      <c r="B137" s="13"/>
+      <c r="C137" s="13"/>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" s="14"/>
-      <c r="B138" s="14"/>
-      <c r="C138" s="14"/>
+      <c r="A138" s="13"/>
+      <c r="B138" s="13"/>
+      <c r="C138" s="13"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" s="14"/>
-      <c r="B139" s="14"/>
-      <c r="C139" s="14"/>
+      <c r="A139" s="13"/>
+      <c r="B139" s="13"/>
+      <c r="C139" s="13"/>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" s="14"/>
-      <c r="B140" s="14"/>
-      <c r="C140" s="14"/>
+      <c r="A140" s="13"/>
+      <c r="B140" s="13"/>
+      <c r="C140" s="13"/>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" s="14"/>
-      <c r="B141" s="14"/>
-      <c r="C141" s="14"/>
+      <c r="A141" s="13"/>
+      <c r="B141" s="13"/>
+      <c r="C141" s="13"/>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A142" s="14"/>
-      <c r="B142" s="14"/>
-      <c r="C142" s="14"/>
+      <c r="A142" s="13"/>
+      <c r="B142" s="13"/>
+      <c r="C142" s="13"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A143" s="14"/>
-      <c r="B143" s="14"/>
-      <c r="C143" s="14"/>
+      <c r="A143" s="13"/>
+      <c r="B143" s="13"/>
+      <c r="C143" s="13"/>
       <c r="E143" s="5"/>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A144" s="14"/>
-      <c r="B144" s="14"/>
-      <c r="C144" s="14"/>
+      <c r="A144" s="13"/>
+      <c r="B144" s="13"/>
+      <c r="C144" s="13"/>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A145" s="14"/>
-      <c r="B145" s="14"/>
-      <c r="C145" s="14"/>
+      <c r="A145" s="13"/>
+      <c r="B145" s="13"/>
+      <c r="C145" s="13"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" s="14"/>
-      <c r="B146" s="14"/>
-      <c r="C146" s="14"/>
+      <c r="A146" s="13"/>
+      <c r="B146" s="13"/>
+      <c r="C146" s="13"/>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" s="14"/>
-      <c r="B147" s="14"/>
-      <c r="C147" s="14"/>
+      <c r="A147" s="13"/>
+      <c r="B147" s="13"/>
+      <c r="C147" s="13"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="14"/>
-      <c r="B148" s="14"/>
-      <c r="C148" s="14"/>
+      <c r="A148" s="13"/>
+      <c r="B148" s="13"/>
+      <c r="C148" s="13"/>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="14"/>
-      <c r="B149" s="14"/>
-      <c r="C149" s="14"/>
+      <c r="A149" s="13"/>
+      <c r="B149" s="13"/>
+      <c r="C149" s="13"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" s="14"/>
-      <c r="B150" s="14"/>
-      <c r="C150" s="14"/>
+      <c r="A150" s="13"/>
+      <c r="B150" s="13"/>
+      <c r="C150" s="13"/>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" s="14"/>
-      <c r="B151" s="14"/>
-      <c r="C151" s="14"/>
+      <c r="A151" s="13"/>
+      <c r="B151" s="13"/>
+      <c r="C151" s="13"/>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" s="14"/>
-      <c r="B152" s="14"/>
-      <c r="C152" s="14"/>
+      <c r="A152" s="13"/>
+      <c r="B152" s="13"/>
+      <c r="C152" s="13"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A153" s="14"/>
-      <c r="B153" s="14"/>
-      <c r="C153" s="14"/>
+      <c r="A153" s="13"/>
+      <c r="B153" s="13"/>
+      <c r="C153" s="13"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" s="14"/>
-      <c r="B154" s="14"/>
-      <c r="C154" s="14"/>
+      <c r="A154" s="13"/>
+      <c r="B154" s="13"/>
+      <c r="C154" s="13"/>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" s="14"/>
-      <c r="B155" s="14"/>
-      <c r="C155" s="14"/>
+      <c r="A155" s="13"/>
+      <c r="B155" s="13"/>
+      <c r="C155" s="13"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" s="14"/>
-      <c r="B156" s="14"/>
-      <c r="C156" s="14"/>
+      <c r="A156" s="13"/>
+      <c r="B156" s="13"/>
+      <c r="C156" s="13"/>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" s="14"/>
-      <c r="B157" s="14"/>
-      <c r="C157" s="14"/>
+      <c r="A157" s="13"/>
+      <c r="B157" s="13"/>
+      <c r="C157" s="13"/>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" s="14"/>
-      <c r="B158" s="14"/>
-      <c r="C158" s="14"/>
+      <c r="A158" s="13"/>
+      <c r="B158" s="13"/>
+      <c r="C158" s="13"/>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" s="14"/>
-      <c r="B159" s="14"/>
-      <c r="C159" s="14"/>
+      <c r="A159" s="13"/>
+      <c r="B159" s="13"/>
+      <c r="C159" s="13"/>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A160" s="14"/>
-      <c r="B160" s="14"/>
-      <c r="C160" s="14"/>
+      <c r="A160" s="13"/>
+      <c r="B160" s="13"/>
+      <c r="C160" s="13"/>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" s="14"/>
-      <c r="B161" s="14"/>
-      <c r="C161" s="14"/>
+      <c r="A161" s="13"/>
+      <c r="B161" s="13"/>
+      <c r="C161" s="13"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" s="14"/>
-      <c r="B162" s="14"/>
-      <c r="C162" s="14"/>
+      <c r="A162" s="13"/>
+      <c r="B162" s="13"/>
+      <c r="C162" s="13"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" s="14"/>
-      <c r="B163" s="14"/>
-      <c r="C163" s="14"/>
+      <c r="A163" s="13"/>
+      <c r="B163" s="13"/>
+      <c r="C163" s="13"/>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" s="14"/>
-      <c r="B164" s="14"/>
-      <c r="C164" s="14"/>
+      <c r="A164" s="13"/>
+      <c r="B164" s="13"/>
+      <c r="C164" s="13"/>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A165" s="14"/>
-      <c r="B165" s="14"/>
-      <c r="C165" s="14"/>
+      <c r="A165" s="13"/>
+      <c r="B165" s="13"/>
+      <c r="C165" s="13"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" s="14"/>
-      <c r="B166" s="14"/>
-      <c r="C166" s="14"/>
+      <c r="A166" s="13"/>
+      <c r="B166" s="13"/>
+      <c r="C166" s="13"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" s="14"/>
-      <c r="B167" s="14"/>
-      <c r="C167" s="14"/>
+      <c r="A167" s="13"/>
+      <c r="B167" s="13"/>
+      <c r="C167" s="13"/>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" s="14"/>
-      <c r="B168" s="14"/>
-      <c r="C168" s="14"/>
+      <c r="A168" s="13"/>
+      <c r="B168" s="13"/>
+      <c r="C168" s="13"/>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169" s="14"/>
-      <c r="B169" s="14"/>
-      <c r="C169" s="14"/>
+      <c r="A169" s="13"/>
+      <c r="B169" s="13"/>
+      <c r="C169" s="13"/>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" s="14"/>
-      <c r="B170" s="14"/>
-      <c r="C170" s="14"/>
+      <c r="A170" s="13"/>
+      <c r="B170" s="13"/>
+      <c r="C170" s="13"/>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" s="14"/>
-      <c r="B171" s="14"/>
-      <c r="C171" s="14"/>
+      <c r="A171" s="13"/>
+      <c r="B171" s="13"/>
+      <c r="C171" s="13"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="14"/>
-      <c r="B172" s="14"/>
-      <c r="C172" s="14"/>
+      <c r="A172" s="13"/>
+      <c r="B172" s="13"/>
+      <c r="C172" s="13"/>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173" s="14"/>
-      <c r="B173" s="14"/>
-      <c r="C173" s="14"/>
+      <c r="A173" s="13"/>
+      <c r="B173" s="13"/>
+      <c r="C173" s="13"/>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="14"/>
-      <c r="B174" s="14"/>
-      <c r="C174" s="14"/>
+      <c r="A174" s="13"/>
+      <c r="B174" s="13"/>
+      <c r="C174" s="13"/>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" s="14"/>
-      <c r="B175" s="14"/>
-      <c r="C175" s="14"/>
+      <c r="A175" s="13"/>
+      <c r="B175" s="13"/>
+      <c r="C175" s="13"/>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" s="14"/>
-      <c r="B176" s="14"/>
-      <c r="C176" s="14"/>
+      <c r="A176" s="13"/>
+      <c r="B176" s="13"/>
+      <c r="C176" s="13"/>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A177" s="14"/>
-      <c r="B177" s="14"/>
-      <c r="C177" s="14"/>
+      <c r="A177" s="13"/>
+      <c r="B177" s="13"/>
+      <c r="C177" s="13"/>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A178" s="14"/>
-      <c r="B178" s="14"/>
-      <c r="C178" s="14"/>
+      <c r="A178" s="13"/>
+      <c r="B178" s="13"/>
+      <c r="C178" s="13"/>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" s="14"/>
-      <c r="B179" s="14"/>
-      <c r="C179" s="14"/>
+      <c r="A179" s="13"/>
+      <c r="B179" s="13"/>
+      <c r="C179" s="13"/>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A180" s="14"/>
-      <c r="B180" s="14"/>
-      <c r="C180" s="14"/>
+      <c r="A180" s="13"/>
+      <c r="B180" s="13"/>
+      <c r="C180" s="13"/>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A181" s="14"/>
-      <c r="B181" s="14"/>
-      <c r="C181" s="14"/>
+      <c r="A181" s="13"/>
+      <c r="B181" s="13"/>
+      <c r="C181" s="13"/>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A182" s="13"/>
-      <c r="B182" s="13"/>
-      <c r="C182" s="13"/>
       <c r="D182" s="6"/>
       <c r="E182" s="7"/>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A183" s="13"/>
-      <c r="B183" s="13"/>
-      <c r="C183" s="13"/>
       <c r="D183" s="6"/>
       <c r="E183" s="7"/>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A184" s="13"/>
-      <c r="B184" s="13"/>
-      <c r="C184" s="13"/>
       <c r="D184" s="6"/>
       <c r="E184" s="7"/>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A185" s="13"/>
-      <c r="B185" s="13"/>
-      <c r="C185" s="13"/>
       <c r="D185" s="6"/>
       <c r="E185" s="7"/>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A186" s="13"/>
-      <c r="B186" s="13"/>
-      <c r="C186" s="13"/>
       <c r="D186" s="6"/>
       <c r="E186" s="7"/>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A187" s="13"/>
-      <c r="B187" s="13"/>
-      <c r="C187" s="13"/>
       <c r="D187" s="6"/>
       <c r="E187" s="7"/>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A188" s="13"/>
-      <c r="B188" s="13"/>
-      <c r="C188" s="13"/>
       <c r="D188" s="6"/>
       <c r="E188" s="7"/>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A189" s="13"/>
-      <c r="B189" s="13"/>
-      <c r="C189" s="13"/>
       <c r="D189" s="6"/>
       <c r="E189" s="7"/>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A190" s="13"/>
-      <c r="B190" s="13"/>
-      <c r="C190" s="13"/>
       <c r="D190" s="6"/>
       <c r="E190" s="7"/>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A191" s="13"/>
-      <c r="B191" s="13"/>
-      <c r="C191" s="13"/>
       <c r="D191" s="6"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A192" s="13"/>
-      <c r="B192" s="13"/>
-      <c r="C192" s="13"/>
       <c r="D192" s="6"/>
       <c r="E192" s="7"/>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A193" s="13"/>
-      <c r="B193" s="13"/>
-      <c r="C193" s="13"/>
+    <row r="193" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D193" s="6"/>
       <c r="E193" s="7"/>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A194" s="13"/>
-      <c r="B194" s="13"/>
-      <c r="C194" s="13"/>
+    <row r="194" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D194" s="6"/>
       <c r="E194" s="7"/>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A195" s="13"/>
-      <c r="B195" s="13"/>
-      <c r="C195" s="13"/>
+    <row r="195" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D195" s="6"/>
       <c r="E195" s="7"/>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A196" s="13"/>
-      <c r="B196" s="13"/>
-      <c r="C196" s="13"/>
+    <row r="196" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D196" s="6"/>
       <c r="E196" s="7"/>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A197" s="13"/>
-      <c r="B197" s="13"/>
-      <c r="C197" s="13"/>
+    <row r="197" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D197" s="6"/>
       <c r="E197" s="7"/>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A198" s="13"/>
-      <c r="B198" s="13"/>
-      <c r="C198" s="13"/>
+    <row r="198" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D198" s="6"/>
       <c r="E198" s="7"/>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A199" s="13"/>
-      <c r="B199" s="13"/>
-      <c r="C199" s="13"/>
+    <row r="199" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D199" s="6"/>
       <c r="E199" s="7"/>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A200" s="13"/>
-      <c r="B200" s="13"/>
-      <c r="C200" s="13"/>
+    <row r="200" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D200" s="6"/>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A201" s="13"/>
-      <c r="B201" s="13"/>
-      <c r="C201" s="13"/>
+    <row r="201" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D201" s="6"/>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A202" s="13"/>
-      <c r="B202" s="13"/>
-      <c r="C202" s="13"/>
+    <row r="202" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D202" s="6"/>
       <c r="E202" s="7"/>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A203" s="13"/>
-      <c r="B203" s="13"/>
-      <c r="C203" s="13"/>
+    <row r="203" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D203" s="6"/>
       <c r="E203" s="7"/>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A204" s="13"/>
-      <c r="B204" s="13"/>
-      <c r="C204" s="13"/>
+    <row r="204" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D204" s="6"/>
       <c r="E204" s="7"/>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A205" s="13"/>
-      <c r="B205" s="13"/>
-      <c r="C205" s="13"/>
+    <row r="205" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D205" s="6"/>
       <c r="E205" s="7"/>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A206" s="13"/>
-      <c r="B206" s="13"/>
-      <c r="C206" s="13"/>
+    <row r="206" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D206" s="6"/>
       <c r="E206" s="7"/>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A207" s="13"/>
-      <c r="B207" s="13"/>
-      <c r="C207" s="13"/>
+    <row r="207" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D207" s="6"/>
       <c r="E207" s="7"/>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A208" s="13"/>
-      <c r="B208" s="13"/>
-      <c r="C208" s="13"/>
+    <row r="208" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D208" s="6"/>
       <c r="E208" s="7"/>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A209" s="13"/>
-      <c r="B209" s="13"/>
-      <c r="C209" s="13"/>
+    <row r="209" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D209" s="6"/>
       <c r="E209" s="7"/>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A210" s="13"/>
-      <c r="B210" s="13"/>
-      <c r="C210" s="13"/>
+    <row r="210" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D210" s="6"/>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A211" s="13"/>
-      <c r="B211" s="13"/>
-      <c r="C211" s="13"/>
+    <row r="211" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D211" s="6"/>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A212" s="13"/>
-      <c r="B212" s="13"/>
-      <c r="C212" s="13"/>
+    <row r="212" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D212" s="6"/>
       <c r="E212" s="7"/>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A213" s="13"/>
-      <c r="B213" s="13"/>
-      <c r="C213" s="13"/>
+    <row r="213" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D213" s="6"/>
       <c r="E213" s="7"/>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A214" s="13"/>
-      <c r="B214" s="13"/>
-      <c r="C214" s="13"/>
+    <row r="214" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D214" s="6"/>
       <c r="E214" s="7"/>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A215" s="13"/>
-      <c r="B215" s="13"/>
-      <c r="C215" s="13"/>
+    <row r="215" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D215" s="6"/>
       <c r="E215" s="7"/>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A216" s="13"/>
-      <c r="B216" s="13"/>
-      <c r="C216" s="13"/>
+    <row r="216" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D216" s="6"/>
       <c r="E216" s="7"/>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A217" s="13"/>
-      <c r="B217" s="13"/>
-      <c r="C217" s="13"/>
+    <row r="217" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D217" s="6"/>
       <c r="E217" s="7"/>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A218" s="13"/>
-      <c r="B218" s="13"/>
-      <c r="C218" s="13"/>
+    <row r="218" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D218" s="6"/>
       <c r="E218" s="7"/>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A219" s="13"/>
-      <c r="B219" s="13"/>
-      <c r="C219" s="13"/>
+    <row r="219" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D219" s="6"/>
       <c r="E219" s="7"/>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A220" s="13"/>
-      <c r="B220" s="13"/>
-      <c r="C220" s="13"/>
+    <row r="220" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D220" s="6"/>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A221" s="13"/>
-      <c r="B221" s="13"/>
-      <c r="C221" s="13"/>
+    <row r="221" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D221" s="6"/>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A222" s="13"/>
-      <c r="B222" s="13"/>
-      <c r="C222" s="13"/>
+    <row r="222" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D222" s="6"/>
       <c r="E222" s="7"/>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A223" s="13"/>
-      <c r="B223" s="13"/>
-      <c r="C223" s="13"/>
+    <row r="223" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D223" s="6"/>
       <c r="E223" s="7"/>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A224" s="13"/>
-      <c r="B224" s="13"/>
-      <c r="C224" s="13"/>
+    <row r="224" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D224" s="6"/>
       <c r="E224" s="7"/>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A225" s="13"/>
-      <c r="B225" s="13"/>
-      <c r="C225" s="13"/>
+    <row r="225" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D225" s="6"/>
       <c r="E225" s="7"/>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A226" s="13"/>
-      <c r="B226" s="13"/>
-      <c r="C226" s="13"/>
+    <row r="226" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D226" s="6"/>
       <c r="E226" s="7"/>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A227" s="13"/>
-      <c r="B227" s="13"/>
-      <c r="C227" s="13"/>
+    <row r="227" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D227" s="6"/>
       <c r="E227" s="7"/>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A228" s="13"/>
-      <c r="B228" s="13"/>
-      <c r="C228" s="13"/>
+    <row r="228" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D228" s="6"/>
       <c r="E228" s="7"/>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A229" s="13"/>
-      <c r="B229" s="13"/>
-      <c r="C229" s="13"/>
+    <row r="229" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D229" s="6"/>
       <c r="E229" s="7"/>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A230" s="13"/>
-      <c r="B230" s="13"/>
-      <c r="C230" s="13"/>
+    <row r="230" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D230" s="6"/>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A231" s="13"/>
-      <c r="B231" s="13"/>
-      <c r="C231" s="13"/>
+    <row r="231" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D231" s="6"/>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A232" s="13"/>
-      <c r="B232" s="13"/>
-      <c r="C232" s="13"/>
+    <row r="232" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D232" s="6"/>
       <c r="E232" s="7"/>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A233" s="13"/>
-      <c r="B233" s="13"/>
-      <c r="C233" s="13"/>
+    <row r="233" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D233" s="6"/>
       <c r="E233" s="7"/>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A234" s="13"/>
-      <c r="B234" s="13"/>
-      <c r="C234" s="13"/>
+    <row r="234" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D234" s="6"/>
       <c r="E234" s="7"/>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A235" s="13"/>
-      <c r="B235" s="13"/>
-      <c r="C235" s="13"/>
+    <row r="235" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D235" s="6"/>
       <c r="E235" s="7"/>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A236" s="13"/>
-      <c r="B236" s="13"/>
-      <c r="C236" s="13"/>
+    <row r="236" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D236" s="6"/>
       <c r="E236" s="7"/>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A237" s="13"/>
-      <c r="B237" s="13"/>
-      <c r="C237" s="13"/>
+    <row r="237" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D237" s="6"/>
       <c r="E237" s="7"/>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A238" s="13"/>
-      <c r="B238" s="13"/>
-      <c r="C238" s="13"/>
+    <row r="238" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D238" s="6"/>
       <c r="E238" s="7"/>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A239" s="13"/>
-      <c r="B239" s="13"/>
-      <c r="C239" s="13"/>
+    <row r="239" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D239" s="6"/>
       <c r="E239" s="7"/>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A240" s="13"/>
-      <c r="B240" s="13"/>
-      <c r="C240" s="13"/>
+    <row r="240" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D240" s="6"/>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A241" s="13"/>
-      <c r="B241" s="13"/>
-      <c r="C241" s="13"/>
+    <row r="241" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D241" s="6"/>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A242" s="13"/>
-      <c r="B242" s="13"/>
-      <c r="C242" s="13"/>
+    <row r="242" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D242" s="6"/>
       <c r="E242" s="7"/>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A243" s="13"/>
-      <c r="B243" s="13"/>
-      <c r="C243" s="13"/>
+    <row r="243" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D243" s="6"/>
       <c r="E243" s="7"/>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A244" s="13"/>
-      <c r="B244" s="13"/>
-      <c r="C244" s="13"/>
+    <row r="244" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D244" s="6"/>
       <c r="E244" s="7"/>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A245" s="13"/>
-      <c r="B245" s="13"/>
-      <c r="C245" s="13"/>
+    <row r="245" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D245" s="6"/>
       <c r="E245" s="7"/>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A246" s="13"/>
-      <c r="B246" s="13"/>
-      <c r="C246" s="13"/>
+    <row r="246" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D246" s="6"/>
       <c r="E246" s="7"/>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A247" s="13"/>
-      <c r="B247" s="13"/>
-      <c r="C247" s="13"/>
+    <row r="247" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D247" s="6"/>
       <c r="E247" s="7"/>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A248" s="13"/>
-      <c r="B248" s="13"/>
-      <c r="C248" s="13"/>
+    <row r="248" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D248" s="6"/>
       <c r="E248" s="8"/>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A249" s="13"/>
-      <c r="B249" s="13"/>
-      <c r="C249" s="13"/>
+    <row r="249" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D249" s="6"/>
       <c r="E249" s="7"/>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A250" s="13"/>
-      <c r="B250" s="13"/>
-      <c r="C250" s="13"/>
+    <row r="250" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D250" s="6"/>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A251" s="13"/>
-      <c r="B251" s="13"/>
-      <c r="C251" s="13"/>
+    <row r="251" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D251" s="6"/>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A252" s="13"/>
-      <c r="B252" s="13"/>
-      <c r="C252" s="13"/>
+    <row r="252" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D252" s="6"/>
       <c r="E252" s="7"/>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A253" s="13"/>
-      <c r="B253" s="13"/>
-      <c r="C253" s="13"/>
+    <row r="253" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D253" s="6"/>
       <c r="E253" s="7"/>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A254" s="13"/>
-      <c r="B254" s="13"/>
-      <c r="C254" s="13"/>
+    <row r="254" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D254" s="6"/>
       <c r="E254" s="7"/>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A255" s="13"/>
-      <c r="B255" s="13"/>
-      <c r="C255" s="13"/>
+    <row r="255" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D255" s="6"/>
       <c r="E255" s="7"/>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A256" s="13"/>
-      <c r="B256" s="13"/>
-      <c r="C256" s="13"/>
+    <row r="256" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D256" s="6"/>
       <c r="E256" s="7"/>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A257" s="13"/>
-      <c r="B257" s="13"/>
-      <c r="C257" s="13"/>
+    <row r="257" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D257" s="6"/>
       <c r="E257" s="7"/>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A258" s="13"/>
-      <c r="B258" s="13"/>
-      <c r="C258" s="13"/>
+    <row r="258" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D258" s="6"/>
       <c r="E258" s="7"/>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A259" s="13"/>
-      <c r="B259" s="13"/>
-      <c r="C259" s="13"/>
+    <row r="259" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D259" s="6"/>
       <c r="E259" s="7"/>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A260" s="13"/>
-      <c r="B260" s="13"/>
-      <c r="C260" s="13"/>
+    <row r="260" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D260" s="6"/>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A261" s="13"/>
-      <c r="B261" s="13"/>
-      <c r="C261" s="13"/>
+    <row r="261" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D261" s="6"/>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A262" s="13"/>
-      <c r="B262" s="13"/>
-      <c r="C262" s="13"/>
+    <row r="262" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D262" s="6"/>
       <c r="E262" s="7"/>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A263" s="13"/>
-      <c r="B263" s="13"/>
-      <c r="C263" s="13"/>
+    <row r="263" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D263" s="6"/>
       <c r="E263" s="7"/>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A264" s="13"/>
-      <c r="B264" s="13"/>
-      <c r="C264" s="13"/>
+    <row r="264" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D264" s="6"/>
       <c r="E264" s="7"/>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A265" s="13"/>
-      <c r="B265" s="13"/>
-      <c r="C265" s="13"/>
+    <row r="265" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D265" s="6"/>
       <c r="E265" s="7"/>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A266" s="13"/>
-      <c r="B266" s="13"/>
-      <c r="C266" s="13"/>
+    <row r="266" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D266" s="6"/>
       <c r="E266" s="7"/>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A267" s="13"/>
-      <c r="B267" s="13"/>
-      <c r="C267" s="13"/>
+    <row r="267" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D267" s="6"/>
       <c r="E267" s="7"/>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A268" s="13"/>
-      <c r="B268" s="13"/>
-      <c r="C268" s="13"/>
+    <row r="268" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D268" s="6"/>
       <c r="E268" s="7"/>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A269" s="13"/>
-      <c r="B269" s="13"/>
-      <c r="C269" s="13"/>
+    <row r="269" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D269" s="6"/>
       <c r="E269" s="7"/>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A270" s="13"/>
-      <c r="B270" s="13"/>
-      <c r="C270" s="13"/>
+    <row r="270" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D270" s="6"/>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A271" s="13"/>
-      <c r="B271" s="13"/>
-      <c r="C271" s="13"/>
+    <row r="271" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D271" s="6"/>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A272" s="13"/>
-      <c r="B272" s="13"/>
-      <c r="C272" s="13"/>
+    <row r="272" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D272" s="6"/>
       <c r="E272" s="7"/>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A273" s="13"/>
-      <c r="B273" s="13"/>
-      <c r="C273" s="13"/>
+    <row r="273" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D273" s="6"/>
       <c r="E273" s="7"/>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A274" s="13"/>
-      <c r="B274" s="13"/>
-      <c r="C274" s="13"/>
+    <row r="274" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D274" s="6"/>
       <c r="E274" s="7"/>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A275" s="13"/>
-      <c r="B275" s="13"/>
-      <c r="C275" s="13"/>
+    <row r="275" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D275" s="6"/>
       <c r="E275" s="7"/>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A276" s="13"/>
-      <c r="B276" s="13"/>
-      <c r="C276" s="13"/>
+    <row r="276" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D276" s="6"/>
       <c r="E276" s="7"/>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A277" s="13"/>
-      <c r="B277" s="13"/>
-      <c r="C277" s="13"/>
+    <row r="277" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D277" s="6"/>
       <c r="E277" s="7"/>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A278" s="13"/>
-      <c r="B278" s="13"/>
-      <c r="C278" s="13"/>
+    <row r="278" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D278" s="6"/>
       <c r="E278" s="7"/>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A279" s="13"/>
-      <c r="B279" s="13"/>
-      <c r="C279" s="13"/>
+    <row r="279" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D279" s="6"/>
       <c r="E279" s="7"/>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A280" s="13"/>
-      <c r="B280" s="13"/>
-      <c r="C280" s="13"/>
+    <row r="280" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D280" s="6"/>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A281" s="13"/>
-      <c r="B281" s="13"/>
-      <c r="C281" s="13"/>
+    <row r="281" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D281" s="6"/>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A282" s="13"/>
-      <c r="B282" s="13"/>
-      <c r="C282" s="13"/>
+    <row r="282" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D282" s="6"/>
       <c r="E282" s="7"/>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A283" s="13"/>
-      <c r="B283" s="13"/>
-      <c r="C283" s="13"/>
+    <row r="283" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D283" s="6"/>
       <c r="E283" s="7"/>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A284" s="13"/>
-      <c r="B284" s="13"/>
-      <c r="C284" s="13"/>
+    <row r="284" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D284" s="6"/>
       <c r="E284" s="7"/>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A285" s="13"/>
-      <c r="B285" s="13"/>
-      <c r="C285" s="13"/>
+    <row r="285" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D285" s="6"/>
       <c r="E285" s="7"/>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A286" s="13"/>
-      <c r="B286" s="13"/>
-      <c r="C286" s="13"/>
+    <row r="286" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D286" s="6"/>
       <c r="E286" s="7"/>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A287" s="13"/>
-      <c r="B287" s="13"/>
-      <c r="C287" s="13"/>
+    <row r="287" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D287" s="6"/>
       <c r="E287" s="7"/>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A288" s="13"/>
-      <c r="B288" s="13"/>
-      <c r="C288" s="13"/>
+    <row r="288" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D288" s="6"/>
       <c r="E288" s="7"/>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A289" s="13"/>
-      <c r="B289" s="13"/>
-      <c r="C289" s="13"/>
+    <row r="289" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D289" s="6"/>
       <c r="E289" s="7"/>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A290" s="13"/>
-      <c r="B290" s="13"/>
-      <c r="C290" s="13"/>
+    <row r="290" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D290" s="6"/>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A291" s="13"/>
-      <c r="B291" s="13"/>
-      <c r="C291" s="13"/>
+    <row r="291" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D291" s="6"/>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A292" s="13"/>
-      <c r="B292" s="13"/>
-      <c r="C292" s="13"/>
+    <row r="292" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D292" s="6"/>
       <c r="E292" s="7"/>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A293" s="13"/>
-      <c r="B293" s="13"/>
-      <c r="C293" s="13"/>
+    <row r="293" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D293" s="6"/>
       <c r="E293" s="7"/>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A294" s="13"/>
-      <c r="B294" s="13"/>
-      <c r="C294" s="13"/>
+    <row r="294" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D294" s="6"/>
       <c r="E294" s="7"/>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A295" s="13"/>
-      <c r="B295" s="13"/>
-      <c r="C295" s="13"/>
+    <row r="295" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D295" s="6"/>
       <c r="E295" s="7"/>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A296" s="13"/>
-      <c r="B296" s="13"/>
-      <c r="C296" s="13"/>
+    <row r="296" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D296" s="6"/>
       <c r="E296" s="7"/>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A297" s="13"/>
-      <c r="B297" s="13"/>
-      <c r="C297" s="13"/>
+    <row r="297" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D297" s="6"/>
       <c r="E297" s="7"/>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A298" s="13"/>
-      <c r="B298" s="13"/>
-      <c r="C298" s="13"/>
+    <row r="298" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D298" s="6"/>
       <c r="E298" s="7"/>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A299" s="13"/>
-      <c r="B299" s="13"/>
-      <c r="C299" s="13"/>
+    <row r="299" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D299" s="6"/>
       <c r="E299" s="7"/>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A300" s="13"/>
-      <c r="B300" s="13"/>
-      <c r="C300" s="13"/>
+    <row r="300" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D300" s="6"/>
       <c r="E300" s="7"/>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A301" s="13"/>
-      <c r="B301" s="13"/>
-      <c r="C301" s="13"/>
+    <row r="301" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D301" s="6"/>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A302" s="13"/>
-      <c r="B302" s="13"/>
-      <c r="C302" s="13"/>
+    <row r="302" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D302" s="6"/>
       <c r="E302" s="7"/>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A303" s="13"/>
-      <c r="B303" s="13"/>
-      <c r="C303" s="13"/>
+    <row r="303" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D303" s="6"/>
       <c r="E303" s="7"/>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A304" s="13"/>
-      <c r="B304" s="13"/>
-      <c r="C304" s="13"/>
+    <row r="304" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D304" s="6"/>
       <c r="E304" s="7"/>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A305" s="13"/>
-      <c r="B305" s="13"/>
-      <c r="C305" s="13"/>
+    <row r="305" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D305" s="6"/>
       <c r="E305" s="7"/>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A306" s="13"/>
-      <c r="B306" s="13"/>
-      <c r="C306" s="13"/>
+    <row r="306" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D306" s="6"/>
       <c r="E306" s="7"/>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A307" s="13"/>
-      <c r="B307" s="13"/>
-      <c r="C307" s="13"/>
+    <row r="307" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D307" s="6"/>
       <c r="E307" s="7"/>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A308" s="13"/>
-      <c r="B308" s="13"/>
-      <c r="C308" s="13"/>
+    <row r="308" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D308" s="6"/>
       <c r="E308" s="7"/>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A309" s="13"/>
-      <c r="B309" s="13"/>
-      <c r="C309" s="13"/>
+    <row r="309" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D309" s="6"/>
       <c r="E309" s="7"/>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A310" s="13"/>
-      <c r="B310" s="13"/>
-      <c r="C310" s="13"/>
+    <row r="310" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D310" s="6"/>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A311" s="13"/>
-      <c r="B311" s="13"/>
-      <c r="C311" s="13"/>
+    <row r="311" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D311" s="6"/>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A312" s="13"/>
-      <c r="B312" s="13"/>
-      <c r="C312" s="13"/>
+    <row r="312" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D312" s="6"/>
       <c r="E312" s="7"/>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A313" s="13"/>
-      <c r="B313" s="13"/>
-      <c r="C313" s="13"/>
+    <row r="313" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D313" s="6"/>
       <c r="E313" s="7"/>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A314" s="13"/>
-      <c r="B314" s="13"/>
-      <c r="C314" s="13"/>
+    <row r="314" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D314" s="6"/>
       <c r="E314" s="7"/>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A315" s="13"/>
-      <c r="B315" s="13"/>
-      <c r="C315" s="13"/>
+    <row r="315" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D315" s="6"/>
       <c r="E315" s="7"/>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A316" s="13"/>
-      <c r="B316" s="13"/>
-      <c r="C316" s="13"/>
+    <row r="316" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D316" s="6"/>
       <c r="E316" s="7"/>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A317" s="13"/>
-      <c r="B317" s="13"/>
-      <c r="C317" s="13"/>
+    <row r="317" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D317" s="6"/>
       <c r="E317" s="7"/>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A318" s="13"/>
-      <c r="B318" s="13"/>
-      <c r="C318" s="13"/>
+    <row r="318" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D318" s="6"/>
       <c r="E318" s="9"/>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A319" s="13"/>
-      <c r="B319" s="13"/>
-      <c r="C319" s="13"/>
+    <row r="319" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D319" s="6"/>
       <c r="E319" s="7"/>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A320" s="13"/>
-      <c r="B320" s="13"/>
-      <c r="C320" s="13"/>
+    <row r="320" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D320" s="6"/>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A321" s="13"/>
-      <c r="B321" s="13"/>
-      <c r="C321" s="13"/>
+    <row r="321" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D321" s="6"/>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A322" s="13"/>
-      <c r="B322" s="13"/>
-      <c r="C322" s="13"/>
+    <row r="322" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D322" s="6"/>
       <c r="E322" s="7"/>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A323" s="13"/>
-      <c r="B323" s="13"/>
-      <c r="C323" s="13"/>
+    <row r="323" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D323" s="6"/>
       <c r="E323" s="7"/>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A324" s="13"/>
-      <c r="B324" s="13"/>
-      <c r="C324" s="13"/>
+    <row r="324" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D324" s="6"/>
       <c r="E324" s="7"/>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A325" s="13"/>
-      <c r="B325" s="13"/>
-      <c r="C325" s="13"/>
+    <row r="325" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D325" s="6"/>
       <c r="E325" s="7"/>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A326" s="13"/>
-      <c r="B326" s="13"/>
-      <c r="C326" s="13"/>
+    <row r="326" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D326" s="6"/>
       <c r="E326" s="7"/>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A327" s="13"/>
-      <c r="B327" s="13"/>
-      <c r="C327" s="13"/>
+    <row r="327" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D327" s="6"/>
       <c r="E327" s="7"/>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A328" s="13"/>
-      <c r="B328" s="13"/>
-      <c r="C328" s="13"/>
+    <row r="328" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D328" s="6"/>
       <c r="E328" s="7"/>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A329" s="13"/>
-      <c r="B329" s="13"/>
-      <c r="C329" s="13"/>
+    <row r="329" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D329" s="6"/>
       <c r="E329" s="7"/>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A330" s="13"/>
-      <c r="B330" s="13"/>
-      <c r="C330" s="13"/>
+    <row r="330" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D330" s="6"/>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A331" s="13"/>
-      <c r="B331" s="13"/>
-      <c r="C331" s="13"/>
+    <row r="331" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D331" s="6"/>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A332" s="13"/>
-      <c r="B332" s="13"/>
-      <c r="C332" s="13"/>
+    <row r="332" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D332" s="6"/>
       <c r="E332" s="7"/>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A333" s="13"/>
-      <c r="B333" s="13"/>
-      <c r="C333" s="13"/>
+    <row r="333" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D333" s="6"/>
       <c r="E333" s="7"/>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A334" s="13"/>
-      <c r="B334" s="13"/>
-      <c r="C334" s="13"/>
+    <row r="334" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D334" s="6"/>
       <c r="E334" s="7"/>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A335" s="13"/>
-      <c r="B335" s="13"/>
-      <c r="C335" s="13"/>
+    <row r="335" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D335" s="6"/>
       <c r="E335" s="7"/>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A336" s="13"/>
-      <c r="B336" s="13"/>
-      <c r="C336" s="13"/>
+    <row r="336" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D336" s="6"/>
       <c r="E336" s="7"/>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A337" s="13"/>
-      <c r="B337" s="13"/>
-      <c r="C337" s="13"/>
+    <row r="337" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D337" s="6"/>
       <c r="E337" s="7"/>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A338" s="13"/>
-      <c r="B338" s="13"/>
-      <c r="C338" s="13"/>
+    <row r="338" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D338" s="6"/>
       <c r="E338" s="7"/>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A339" s="13"/>
-      <c r="B339" s="13"/>
-      <c r="C339" s="13"/>
+    <row r="339" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D339" s="6"/>
       <c r="E339" s="7"/>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A340" s="13"/>
-      <c r="B340" s="13"/>
-      <c r="C340" s="13"/>
+    <row r="340" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D340" s="6"/>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A341" s="13"/>
-      <c r="B341" s="13"/>
-      <c r="C341" s="13"/>
+    <row r="341" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D341" s="6"/>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A342" s="13"/>
-      <c r="B342" s="13"/>
-      <c r="C342" s="13"/>
+    <row r="342" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D342" s="6"/>
       <c r="E342" s="7"/>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A343" s="13"/>
-      <c r="B343" s="13"/>
-      <c r="C343" s="13"/>
+    <row r="343" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D343" s="6"/>
       <c r="E343" s="7"/>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A344" s="13"/>
-      <c r="B344" s="13"/>
-      <c r="C344" s="13"/>
+    <row r="344" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D344" s="6"/>
       <c r="E344" s="7"/>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A345" s="13"/>
-      <c r="B345" s="13"/>
-      <c r="C345" s="13"/>
+    <row r="345" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D345" s="6"/>
       <c r="E345" s="7"/>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A346" s="13"/>
-      <c r="B346" s="13"/>
-      <c r="C346" s="13"/>
+    <row r="346" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D346" s="6"/>
       <c r="E346" s="7"/>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A347" s="13"/>
-      <c r="B347" s="13"/>
-      <c r="C347" s="13"/>
+    <row r="347" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D347" s="6"/>
       <c r="E347" s="7"/>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A348" s="13"/>
-      <c r="B348" s="13"/>
-      <c r="C348" s="13"/>
+    <row r="348" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D348" s="6"/>
       <c r="E348" s="7"/>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A349" s="13"/>
-      <c r="B349" s="13"/>
-      <c r="C349" s="13"/>
+    <row r="349" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D349" s="6"/>
       <c r="E349" s="7"/>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A350" s="13"/>
-      <c r="B350" s="13"/>
-      <c r="C350" s="13"/>
+    <row r="350" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D350" s="6"/>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A351" s="13"/>
-      <c r="B351" s="13"/>
-      <c r="C351" s="13"/>
+    <row r="351" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D351" s="6"/>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A352" s="13"/>
-      <c r="B352" s="13"/>
-      <c r="C352" s="13"/>
+    <row r="352" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D352" s="6"/>
       <c r="E352" s="7"/>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A353" s="13"/>
-      <c r="B353" s="13"/>
-      <c r="C353" s="13"/>
+    <row r="353" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D353" s="6"/>
       <c r="E353" s="7"/>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A354" s="13"/>
-      <c r="B354" s="13"/>
-      <c r="C354" s="13"/>
+    <row r="354" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D354" s="6"/>
       <c r="E354" s="7"/>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A355" s="13"/>
-      <c r="B355" s="13"/>
-      <c r="C355" s="13"/>
+    <row r="355" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D355" s="6"/>
       <c r="E355" s="7"/>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A356" s="13"/>
-      <c r="B356" s="13"/>
-      <c r="C356" s="13"/>
+    <row r="356" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D356" s="6"/>
       <c r="E356" s="7"/>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A357" s="13"/>
-      <c r="B357" s="13"/>
-      <c r="C357" s="13"/>
+    <row r="357" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D357" s="6"/>
       <c r="E357" s="7"/>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A358" s="13"/>
-      <c r="B358" s="13"/>
-      <c r="C358" s="13"/>
+    <row r="358" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D358" s="6"/>
       <c r="E358" s="7"/>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A359" s="13"/>
-      <c r="B359" s="13"/>
-      <c r="C359" s="13"/>
+    <row r="359" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D359" s="6"/>
       <c r="E359" s="7"/>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A360" s="13"/>
-      <c r="B360" s="13"/>
-      <c r="C360" s="13"/>
+    <row r="360" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D360" s="6"/>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A361" s="13"/>
-      <c r="B361" s="13"/>
-      <c r="C361" s="13"/>
+    <row r="361" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D361" s="6"/>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A362" s="13"/>
-      <c r="B362" s="13"/>
-      <c r="C362" s="13"/>
+    <row r="362" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D362" s="6"/>
       <c r="E362" s="7"/>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A363" s="13"/>
-      <c r="B363" s="13"/>
-      <c r="C363" s="13"/>
+    <row r="363" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D363" s="6"/>
       <c r="E363" s="7"/>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A364" s="13"/>
-      <c r="B364" s="13"/>
-      <c r="C364" s="13"/>
+    <row r="364" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D364" s="6"/>
       <c r="E364" s="7"/>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A365" s="13"/>
-      <c r="B365" s="13"/>
-      <c r="C365" s="13"/>
+    <row r="365" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D365" s="6"/>
       <c r="E365" s="7"/>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A366" s="13"/>
-      <c r="B366" s="13"/>
-      <c r="C366" s="13"/>
+    <row r="366" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D366" s="6"/>
       <c r="E366" s="7"/>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A367" s="13"/>
-      <c r="B367" s="13"/>
-      <c r="C367" s="13"/>
+    <row r="367" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D367" s="6"/>
       <c r="E367" s="7"/>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A368" s="13"/>
-      <c r="B368" s="13"/>
-      <c r="C368" s="13"/>
+    <row r="368" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D368" s="6"/>
       <c r="E368" s="7"/>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A369" s="13"/>
-      <c r="B369" s="13"/>
-      <c r="C369" s="13"/>
+    <row r="369" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D369" s="6"/>
       <c r="E369" s="7"/>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A370" s="13"/>
-      <c r="B370" s="13"/>
-      <c r="C370" s="13"/>
+    <row r="370" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D370" s="6"/>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A371" s="13"/>
-      <c r="B371" s="13"/>
-      <c r="C371" s="13"/>
+    <row r="371" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D371" s="6"/>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A372" s="13"/>
-      <c r="B372" s="13"/>
-      <c r="C372" s="13"/>
+    <row r="372" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D372" s="6"/>
       <c r="E372" s="7"/>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A373" s="13"/>
-      <c r="B373" s="13"/>
-      <c r="C373" s="13"/>
+    <row r="373" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D373" s="6"/>
       <c r="E373" s="7"/>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A374" s="13"/>
-      <c r="B374" s="13"/>
-      <c r="C374" s="13"/>
+    <row r="374" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D374" s="6"/>
       <c r="E374" s="7"/>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A375" s="13"/>
-      <c r="B375" s="13"/>
-      <c r="C375" s="13"/>
+    <row r="375" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D375" s="6"/>
       <c r="E375" s="7"/>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A376" s="13"/>
-      <c r="B376" s="13"/>
-      <c r="C376" s="13"/>
+    <row r="376" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D376" s="6"/>
       <c r="E376" s="7"/>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A377" s="13"/>
-      <c r="B377" s="13"/>
-      <c r="C377" s="13"/>
+    <row r="377" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D377" s="6"/>
       <c r="E377" s="7"/>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A378" s="13"/>
-      <c r="B378" s="13"/>
-      <c r="C378" s="13"/>
+    <row r="378" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D378" s="6"/>
       <c r="E378" s="7"/>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A379" s="13"/>
-      <c r="B379" s="13"/>
-      <c r="C379" s="13"/>
+    <row r="379" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D379" s="6"/>
       <c r="E379" s="7"/>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A380" s="13"/>
-      <c r="B380" s="13"/>
-      <c r="C380" s="13"/>
+    <row r="380" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D380" s="6"/>
     </row>
-    <row r="381" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A381" s="13"/>
-      <c r="B381" s="13"/>
-      <c r="C381" s="13"/>
+    <row r="381" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D381" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove unnecessary double quotes
</commit_message>
<xml_diff>
--- a/refair-server/datasets/Few Shot dataset/FSDataset3.xlsx
+++ b/refair-server/datasets/Few Shot dataset/FSDataset3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele\Desktop\SE4AI Project\ReFair-App\refair-server\datasets\Few Shot dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD895AC4-54AD-47A7-B362-F66ADDF5F23E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBEA249-7AB1-4CA1-8C04-6CB1A57BF527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{80773445-FB61-4F04-A882-1600FD96C55A}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -365,9 +365,6 @@
     <t>As a network security analyst, I want to employ techniques for handling imbalanced datasets in machine learning to better detect rare and critical cybersecurity threats, such as zero-day attacks, so that our network remains secure against evolving threats.</t>
   </si>
   <si>
-    <t>As a computer vision researcher, I want to address class imbalance in my dataset so that my model can accurately detect rare visual anomalies in industrial inspection images, ensuring early detection of critical faults and minimizing downtime."</t>
-  </si>
-  <si>
     <t>As a network security analyst, I want to apply keyword extraction in NLP to analyze security incident reports and identify key terms related to potential threats, so that I can prioritize and respond to security incidents effectively.</t>
   </si>
   <si>
@@ -438,6 +435,9 @@
   </si>
   <si>
     <t>As a computer vision researcher, I want to leverage word embedding techniques to enhance image captioning models, so that they can generate more contextually accurate and semantically rich descriptions of visual content.</t>
+  </si>
+  <si>
+    <t>As a computer vision researcher, I want to address class imbalance in my dataset so that my model can accurately detect rare visual anomalies in industrial inspection images, ensuring early detection of critical faults and minimizing downtime.</t>
   </si>
 </sst>
 </file>
@@ -893,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF0B04-8323-4309-B759-D1CDDA1FBB0E}">
   <dimension ref="A1:F381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E101" sqref="E101"/>
+    <sheetView tabSelected="1" topLeftCell="E68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2440,7 +2440,7 @@
         <v>8</v>
       </c>
       <c r="E77" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>26</v>
@@ -2460,7 +2460,7 @@
         <v>19</v>
       </c>
       <c r="E78" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>26</v>
@@ -2480,7 +2480,7 @@
         <v>19</v>
       </c>
       <c r="E79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>26</v>
@@ -2500,7 +2500,7 @@
         <v>9</v>
       </c>
       <c r="E80" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>26</v>
@@ -2520,7 +2520,7 @@
         <v>9</v>
       </c>
       <c r="E81" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>26</v>
@@ -2540,7 +2540,7 @@
         <v>22</v>
       </c>
       <c r="E82" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>26</v>
@@ -2560,7 +2560,7 @@
         <v>22</v>
       </c>
       <c r="E83" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>26</v>
@@ -2580,7 +2580,7 @@
         <v>10</v>
       </c>
       <c r="E84" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>26</v>
@@ -2600,7 +2600,7 @@
         <v>10</v>
       </c>
       <c r="E85" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>26</v>
@@ -2620,7 +2620,7 @@
         <v>11</v>
       </c>
       <c r="E86" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>26</v>
@@ -2640,7 +2640,7 @@
         <v>11</v>
       </c>
       <c r="E87" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>26</v>
@@ -2660,7 +2660,7 @@
         <v>12</v>
       </c>
       <c r="E88" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>26</v>
@@ -2680,7 +2680,7 @@
         <v>12</v>
       </c>
       <c r="E89" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>26</v>
@@ -2700,7 +2700,7 @@
         <v>21</v>
       </c>
       <c r="E90" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>26</v>
@@ -2720,7 +2720,7 @@
         <v>21</v>
       </c>
       <c r="E91" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>26</v>
@@ -2740,7 +2740,7 @@
         <v>13</v>
       </c>
       <c r="E92" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>26</v>
@@ -2760,7 +2760,7 @@
         <v>13</v>
       </c>
       <c r="E93" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>26</v>
@@ -2780,7 +2780,7 @@
         <v>14</v>
       </c>
       <c r="E94" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>26</v>
@@ -2800,7 +2800,7 @@
         <v>14</v>
       </c>
       <c r="E95" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>26</v>
@@ -2820,7 +2820,7 @@
         <v>17</v>
       </c>
       <c r="E96" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>26</v>
@@ -2840,7 +2840,7 @@
         <v>17</v>
       </c>
       <c r="E97" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>26</v>
@@ -2860,7 +2860,7 @@
         <v>4</v>
       </c>
       <c r="E98" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>26</v>
@@ -2880,7 +2880,7 @@
         <v>4</v>
       </c>
       <c r="E99" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>26</v>
@@ -2900,7 +2900,7 @@
         <v>5</v>
       </c>
       <c r="E100" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>26</v>
@@ -2920,7 +2920,7 @@
         <v>5</v>
       </c>
       <c r="E101" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>26</v>

</xml_diff>